<commit_message>
Added items function with seeder
</commit_message>
<xml_diff>
--- a/WorkBreakdown_SuperAngel.xlsx
+++ b/WorkBreakdown_SuperAngel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Wat</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Carousel Dynamisch gemaakt</t>
+  </si>
+  <si>
+    <t>Seeders and migrations</t>
+  </si>
+  <si>
+    <t>Kan meer worden naarmate ik meer data nodig heb</t>
+  </si>
+  <si>
+    <t>Items</t>
   </si>
 </sst>
 </file>
@@ -537,7 +546,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,6 +554,7 @@
     <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -560,7 +570,7 @@
       </c>
       <c r="G1">
         <f>SUM(C24)</f>
-        <v>23.2</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -771,59 +781,78 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="7">
-        <f>SUM(B3:B16)</f>
-        <v>33.700000000000003</v>
+        <f>SUM(B3:B18)</f>
+        <v>35.700000000000003</v>
       </c>
       <c r="C24" s="7">
-        <f>SUM(C3:C16)</f>
-        <v>23.2</v>
+        <f>SUM(C3:C18)</f>
+        <v>25.2</v>
       </c>
       <c r="D24" s="7"/>
     </row>

</xml_diff>

<commit_message>
Added items function with seeder Seeder updated error in migrate fixed All works well now!
</commit_message>
<xml_diff>
--- a/WorkBreakdown_SuperAngel.xlsx
+++ b/WorkBreakdown_SuperAngel.xlsx
@@ -546,7 +546,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
       </c>
       <c r="G1">
         <f>SUM(C24)</f>
-        <v>25.2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -786,10 +786,10 @@
         <v>23</v>
       </c>
       <c r="B17" s="6">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="C17" s="6">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>4</v>
@@ -848,11 +848,11 @@
       </c>
       <c r="B24" s="7">
         <f>SUM(B3:B18)</f>
-        <v>35.700000000000003</v>
+        <v>36.400000000000006</v>
       </c>
       <c r="C24" s="7">
         <f>SUM(C3:C18)</f>
-        <v>25.2</v>
+        <v>26</v>
       </c>
       <c r="D24" s="7"/>
     </row>

</xml_diff>

<commit_message>
Item stocks Cart display Cart add items Some more minor fixes
</commit_message>
<xml_diff>
--- a/WorkBreakdown_SuperAngel.xlsx
+++ b/WorkBreakdown_SuperAngel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Wat</t>
   </si>
@@ -74,34 +74,61 @@
     <t>Mijn gegevens incl update in database</t>
   </si>
   <si>
-    <t>Winkelwagen</t>
+    <t>Categorieen in header en in de shop</t>
+  </si>
+  <si>
+    <t>Winkelwagen library gezocht en toegevoegd</t>
+  </si>
+  <si>
+    <t>ComposerServiceProvider</t>
+  </si>
+  <si>
+    <t>MainComposer</t>
+  </si>
+  <si>
+    <t>Carousel Dynamisch gemaakt</t>
+  </si>
+  <si>
+    <t>Seeders and migrations</t>
+  </si>
+  <si>
+    <t>Kan meer worden naarmate ik meer data nodig heb</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Product pagina</t>
+  </si>
+  <si>
+    <t>Toevoegen aan winkelwagen</t>
+  </si>
+  <si>
+    <t>Producten toevoegen aan winkelwagen</t>
+  </si>
+  <si>
+    <t>Product vooraad</t>
+  </si>
+  <si>
+    <t>Winkelwagen aantal en prijs weergave</t>
+  </si>
+  <si>
+    <t>Winkelwagen weergave</t>
   </si>
   <si>
     <t>Nee</t>
   </si>
   <si>
-    <t>Categorieen in header en in de shop</t>
-  </si>
-  <si>
-    <t>Winkelwagen library gezocht en toegevoegd</t>
-  </si>
-  <si>
-    <t>ComposerServiceProvider</t>
-  </si>
-  <si>
-    <t>MainComposer</t>
-  </si>
-  <si>
-    <t>Carousel Dynamisch gemaakt</t>
-  </si>
-  <si>
-    <t>Seeders and migrations</t>
-  </si>
-  <si>
-    <t>Kan meer worden naarmate ik meer data nodig heb</t>
-  </si>
-  <si>
-    <t>Items</t>
+    <t>Winkelwagen Updaten</t>
+  </si>
+  <si>
+    <t>Winkelwagen verwijderen</t>
+  </si>
+  <si>
+    <t>Winkelwagen product verwijderen</t>
+  </si>
+  <si>
+    <t>Melding voor succesvol toevoegen van product</t>
   </si>
 </sst>
 </file>
@@ -543,19 +570,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.42578125" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -569,8 +597,8 @@
         <v>13</v>
       </c>
       <c r="G1">
-        <f>SUM(C24)</f>
-        <v>26</v>
+        <f>SUM(C34)</f>
+        <v>34.5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -704,22 +732,24 @@
         <v>16</v>
       </c>
       <c r="B11" s="6">
-        <v>10</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.5</v>
+      </c>
       <c r="D11" s="6" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C12" s="6">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>4</v>
@@ -727,7 +757,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="6">
         <v>0.5</v>
@@ -741,7 +771,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6">
         <v>0.5</v>
@@ -755,13 +785,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C15" s="6">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>4</v>
@@ -769,92 +799,220 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="6">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="C17" s="6">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B19" s="6">
         <v>1.5</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C19" s="6">
         <v>1.5</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="D19" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="7">
-        <f>SUM(B3:B18)</f>
-        <v>36.400000000000006</v>
-      </c>
-      <c r="C24" s="7">
-        <f>SUM(C3:C18)</f>
-        <v>26</v>
-      </c>
-      <c r="D24" s="7"/>
+      <c r="B34" s="7">
+        <f>SUM(B3:B27)</f>
+        <v>39.400000000000006</v>
+      </c>
+      <c r="C34" s="7">
+        <f>SUM(C3:C22)</f>
+        <v>34.5</v>
+      </c>
+      <c r="D34" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>